<commit_message>
Draw.io(conceitual) e tabelas BD
</commit_message>
<xml_diff>
--- a/Excel Modelagem.xlsx
+++ b/Excel Modelagem.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\51418943800\Desktop\SPRINT 1\Projeto SP MEDICAL GROUP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\51418943800\Desktop\SPRINT 1\Projeto SP MEDICAL GROUP\SP-MEDICAL-GROUP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>CLINICA</t>
   </si>
@@ -104,9 +104,6 @@
     <t>DESCRIÇÃO</t>
   </si>
   <si>
-    <t>ID_DESCRIÇÃO</t>
-  </si>
-  <si>
     <t>USUARIOS</t>
   </si>
   <si>
@@ -125,13 +122,19 @@
     <t>medcorp</t>
   </si>
   <si>
-    <t>Adm</t>
-  </si>
-  <si>
     <t xml:space="preserve">nulo </t>
   </si>
   <si>
     <t>Pediatria</t>
+  </si>
+  <si>
+    <t>ID_USUARIO</t>
+  </si>
+  <si>
+    <t>Paciente</t>
+  </si>
+  <si>
+    <t>Médico</t>
   </si>
 </sst>
 </file>
@@ -484,17 +487,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.88671875" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
@@ -504,7 +507,7 @@
     <col min="11" max="11" width="13.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -515,7 +518,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -538,12 +541,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
@@ -551,20 +554,20 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="7"/>
       <c r="D5" s="1"/>
       <c r="E5" s="6"/>
       <c r="F5" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -572,11 +575,11 @@
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="F6" s="2" t="s">
         <v>1</v>
       </c>
@@ -584,7 +587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -597,188 +600,196 @@
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="G11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="H10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="4">
-        <v>1</v>
-      </c>
-      <c r="F12" s="4">
-        <v>1</v>
-      </c>
-      <c r="H12" s="3">
-        <v>1</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
-        <v>1</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="3">
+        <v>2</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="H20" s="5" t="s">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="H21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="2" t="s">
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
-        <v>1</v>
-      </c>
-      <c r="B22" s="2">
-        <v>1</v>
-      </c>
-      <c r="C22" s="2">
-        <v>1</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="2">
-        <v>1</v>
-      </c>
-      <c r="H22" s="3">
+      <c r="H22" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>31</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3">
+        <v>1</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>